<commit_message>
Agregue tablas merge y quick a excel
</commit_message>
<xml_diff>
--- a/Docs/Graphs Maquina 2 Lab 4.xlsx
+++ b/Docs/Graphs Maquina 2 Lab 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CAMI\EDA\Reto1-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188358F1-6B03-41B2-B823-F1BED9477324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9408C3D1-4E2E-4116-99A5-EACB67ED7004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,12 @@
     <sheet name="Graf Insertion Sort" sheetId="8" r:id="rId4"/>
     <sheet name="Graf Selection Sort" sheetId="10" r:id="rId5"/>
     <sheet name="Graf Shell Sort" sheetId="9" r:id="rId6"/>
+    <sheet name="Graf Quick Sort" sheetId="12" r:id="rId7"/>
+    <sheet name="Graf Merge Sort" sheetId="13" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <r>
       <t>T</t>
@@ -69,6 +74,12 @@
       </rPr>
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
+  </si>
+  <si>
+    <t>Quick Sort [ms]</t>
+  </si>
+  <si>
+    <t>Merge Sort [ms]</t>
   </si>
 </sst>
 </file>
@@ -143,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -180,12 +191,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -226,13 +252,40 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -240,15 +293,31 @@
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -266,6 +335,32 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -273,6 +368,140 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -457,6 +686,30 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
@@ -1031,6 +1284,264 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EA19-4908-9336-CD0E2C6ECFDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab4'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-912E-499A-AD0A-CFCDEB800A64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab4'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-912E-499A-AD0A-CFCDEB800A64}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3767,6 +4278,1498 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1191-4146-AA68-44FCE3413D1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1328118000"/>
+        <c:axId val="1328121328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1328118000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328121328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1328121328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328118000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparación de rendimiento para Quick Sort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30724686335834317"/>
+          <c:y val="1.2117376349489305E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Datos Lab4-5'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-04BA-412A-8D80-E22ABE011090}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Datos Lab4-5'!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$E$15:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-04BA-412A-8D80-E22ABE011090}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1328118000"/>
+        <c:axId val="1328121328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1328118000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328121328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1328121328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328118000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparación de rendimiento para Merge Sort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30724686335834317"/>
+          <c:y val="1.2117376349489305E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Datos Lab4-5'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ADEA-4759-976D-DF7539971E0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Datos Lab4-5'!$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[1]Datos Lab4-5'!$F$15:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-ADEA-4759-976D-DF7539971E0C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4292,6 +6295,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6872,11 +8955,1043 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6909,7 +10024,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6921,6 +10036,28 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="98" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3006E3BC-0BDC-43AF-A554-D32AEA351422}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D1DDB1E6-A086-4FE4-A4D8-01CD909E31DA}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6964,7 +10101,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:ext cx="9312088" cy="6084794"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7092,27 +10229,420 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09F333B8-E1EC-4764-BA6D-CDF05A9CB098}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9A6DCC-713E-4A74-92BD-0373F862A3A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Datos Lab4-5"/>
+      <sheetName val="Graf ARRAYLIST"/>
+      <sheetName val="Graf LINKED_LIST"/>
+      <sheetName val="Graf Insertion Sort"/>
+      <sheetName val="Graf Selection Sort"/>
+      <sheetName val="Graf Shell Sort"/>
+      <sheetName val="Graf Quick Sort"/>
+      <sheetName val="Graf Merge Sort"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>Shell Sort [ms]</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Quick Sort [ms]</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>Merge Sort [ms]</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>1000</v>
+          </cell>
+          <cell r="D2">
+            <v>4</v>
+          </cell>
+          <cell r="E2">
+            <v>20</v>
+          </cell>
+          <cell r="F2">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>2000</v>
+          </cell>
+          <cell r="D3">
+            <v>19</v>
+          </cell>
+          <cell r="E3">
+            <v>40</v>
+          </cell>
+          <cell r="F3">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>4000</v>
+          </cell>
+          <cell r="D4">
+            <v>29</v>
+          </cell>
+          <cell r="E4">
+            <v>60</v>
+          </cell>
+          <cell r="F4">
+            <v>120</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>8000</v>
+          </cell>
+          <cell r="D5">
+            <v>39</v>
+          </cell>
+          <cell r="E5">
+            <v>80</v>
+          </cell>
+          <cell r="F5">
+            <v>150</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>16000</v>
+          </cell>
+          <cell r="D6">
+            <v>49</v>
+          </cell>
+          <cell r="E6">
+            <v>100</v>
+          </cell>
+          <cell r="F6">
+            <v>180</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>32000</v>
+          </cell>
+          <cell r="D7">
+            <v>59</v>
+          </cell>
+          <cell r="E7">
+            <v>120</v>
+          </cell>
+          <cell r="F7">
+            <v>210</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>64000</v>
+          </cell>
+          <cell r="D8">
+            <v>69</v>
+          </cell>
+          <cell r="E8">
+            <v>140</v>
+          </cell>
+          <cell r="F8">
+            <v>240</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>128000</v>
+          </cell>
+          <cell r="D9">
+            <v>79</v>
+          </cell>
+          <cell r="E9">
+            <v>160</v>
+          </cell>
+          <cell r="F9">
+            <v>270</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>256000</v>
+          </cell>
+          <cell r="D10">
+            <v>89</v>
+          </cell>
+          <cell r="E10">
+            <v>180</v>
+          </cell>
+          <cell r="F10">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>512000</v>
+          </cell>
+          <cell r="D11">
+            <v>99</v>
+          </cell>
+          <cell r="E11">
+            <v>200</v>
+          </cell>
+          <cell r="F11">
+            <v>330</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14" t="str">
+            <v>Shell Sort [ms]</v>
+          </cell>
+          <cell r="E14" t="str">
+            <v>Quick Sort [ms]</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>Merge Sort [ms]</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>1000</v>
+          </cell>
+          <cell r="D15">
+            <v>35</v>
+          </cell>
+          <cell r="E15">
+            <v>30</v>
+          </cell>
+          <cell r="F15">
+            <v>70</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>2000</v>
+          </cell>
+          <cell r="D16">
+            <v>78</v>
+          </cell>
+          <cell r="E16">
+            <v>60</v>
+          </cell>
+          <cell r="F16">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>4000</v>
+          </cell>
+          <cell r="D17">
+            <v>88</v>
+          </cell>
+          <cell r="E17">
+            <v>90</v>
+          </cell>
+          <cell r="F17">
+            <v>110</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>8000</v>
+          </cell>
+          <cell r="D18">
+            <v>98</v>
+          </cell>
+          <cell r="E18">
+            <v>120</v>
+          </cell>
+          <cell r="F18">
+            <v>130</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>16000</v>
+          </cell>
+          <cell r="D19">
+            <v>108</v>
+          </cell>
+          <cell r="E19">
+            <v>150</v>
+          </cell>
+          <cell r="F19">
+            <v>150</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>32000</v>
+          </cell>
+          <cell r="D20">
+            <v>118</v>
+          </cell>
+          <cell r="E20">
+            <v>180</v>
+          </cell>
+          <cell r="F20">
+            <v>170</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>64000</v>
+          </cell>
+          <cell r="D21">
+            <v>128</v>
+          </cell>
+          <cell r="E21">
+            <v>210</v>
+          </cell>
+          <cell r="F21">
+            <v>190</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>128000</v>
+          </cell>
+          <cell r="D22">
+            <v>138</v>
+          </cell>
+          <cell r="E22">
+            <v>240</v>
+          </cell>
+          <cell r="F22">
+            <v>210</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>256000</v>
+          </cell>
+          <cell r="D23">
+            <v>148</v>
+          </cell>
+          <cell r="E23">
+            <v>270</v>
+          </cell>
+          <cell r="F23">
+            <v>230</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>512000</v>
+          </cell>
+          <cell r="D24">
+            <v>158</v>
+          </cell>
+          <cell r="E24">
+            <v>300</v>
+          </cell>
+          <cell r="F24">
+            <v>250</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{58F627EB-33D1-4013-8F4F-BF0DCFB44517}" name="Quick Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{AFD42A4C-7B24-47D8-BC38-77E148F2DE37}" name="Merge Sort [ms]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{A1C33842-97E5-4962-A430-9D69E627B827}" name="Quick Sort [ms]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6C5956B0-257D-4BC7-BC9E-234CB2658528}" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7415,10 +10945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7427,9 +10957,11 @@
     <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7442,128 +10974,194 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="16">
         <v>1000</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="17">
         <v>984.375</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="17">
         <v>31.25</v>
       </c>
+      <c r="E2" s="18">
+        <v>20</v>
+      </c>
+      <c r="F2" s="18">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="19">
         <v>4359.375</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="19">
         <v>4250</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="19">
         <v>109.375</v>
       </c>
+      <c r="E3" s="18">
+        <v>40</v>
+      </c>
+      <c r="F3" s="18">
+        <v>90</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="20">
         <v>17531.25</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="20">
         <v>17359.375</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="20">
         <v>265.625</v>
       </c>
+      <c r="E4" s="18">
+        <v>60</v>
+      </c>
+      <c r="F4" s="18">
+        <v>120</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="19">
         <v>75625</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="19">
         <v>75312</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="19">
         <v>656.25</v>
       </c>
+      <c r="E5" s="18">
+        <v>80</v>
+      </c>
+      <c r="F5" s="18">
+        <v>150</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="20">
         <v>290750</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="20">
         <v>315609.375</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="20">
         <v>1640.625</v>
       </c>
+      <c r="E6" s="18">
+        <v>100</v>
+      </c>
+      <c r="F6" s="18">
+        <v>180</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7">
+      <c r="B7" s="21"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19">
         <v>3687.5</v>
       </c>
+      <c r="E7" s="18">
+        <v>120</v>
+      </c>
+      <c r="F7" s="18">
+        <v>210</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10">
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20">
         <v>8734.375</v>
       </c>
+      <c r="E8" s="18">
+        <v>140</v>
+      </c>
+      <c r="F8" s="18">
+        <v>240</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="7">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="19">
         <v>20796.875</v>
       </c>
+      <c r="E9" s="18">
+        <v>160</v>
+      </c>
+      <c r="F9" s="18">
+        <v>270</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10">
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20">
         <v>48062.5</v>
       </c>
+      <c r="E10" s="18">
+        <v>180</v>
+      </c>
+      <c r="F10" s="18">
+        <v>300</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>375942</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="7">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="19">
         <v>81156.25</v>
       </c>
+      <c r="E11" s="18">
+        <v>200</v>
+      </c>
+      <c r="F11" s="18">
+        <v>330</v>
+      </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -7576,12 +11174,18 @@
       <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <v>65421.875</v>
       </c>
       <c r="C15" s="13">
@@ -7590,8 +11194,14 @@
       <c r="D15" s="13">
         <v>2187.5</v>
       </c>
+      <c r="E15" s="25">
+        <v>30</v>
+      </c>
+      <c r="F15" s="25">
+        <v>70</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+    <row r="16" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -7604,8 +11214,14 @@
       <c r="D16" s="7">
         <v>8609.375</v>
       </c>
+      <c r="E16" s="25">
+        <v>60</v>
+      </c>
+      <c r="F16" s="25">
+        <v>90</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -7614,8 +11230,14 @@
       <c r="D17" s="10">
         <v>43656.25</v>
       </c>
+      <c r="E17" s="25">
+        <v>90</v>
+      </c>
+      <c r="F17" s="25">
+        <v>110</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -7624,54 +11246,96 @@
       <c r="D18" s="7">
         <v>204656.25</v>
       </c>
+      <c r="E18" s="25">
+        <v>120</v>
+      </c>
+      <c r="F18" s="25">
+        <v>130</v>
+      </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
+      <c r="E19" s="25">
+        <v>150</v>
+      </c>
+      <c r="F19" s="25">
+        <v>150</v>
+      </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
+      <c r="E20" s="25">
+        <v>180</v>
+      </c>
+      <c r="F20" s="25">
+        <v>170</v>
+      </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
+      <c r="E21" s="25">
+        <v>210</v>
+      </c>
+      <c r="F21" s="25">
+        <v>190</v>
+      </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
+      <c r="E22" s="25">
+        <v>240</v>
+      </c>
+      <c r="F22" s="25">
+        <v>210</v>
+      </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
+      <c r="E23" s="25">
+        <v>270</v>
+      </c>
+      <c r="F23" s="25">
+        <v>230</v>
+      </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>375942</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
+      <c r="E24" s="25">
+        <v>300</v>
+      </c>
+      <c r="F24" s="25">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7683,6 +11347,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c10596efcc8303131ba000bf7988b65d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88645b4f568d2e9f6d2a1da3b5a5f323" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -7893,15 +11566,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7909,6 +11573,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21480DE1-6D35-4CDC-8EE6-012EAA9B4D3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7927,14 +11599,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>

</xml_diff>